<commit_message>
Script update to include k means
</commit_message>
<xml_diff>
--- a/Survey/Completed Surveys/Results.xlsx
+++ b/Survey/Completed Surveys/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\IdeaProjects\CSC_8639_3.8\Survey\Completed Surveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9405BCF-0CF0-4493-BEDA-224875659560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F884CA-5508-4B91-9991-7D989105CCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10068" yWindow="0" windowWidth="20988" windowHeight="16824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,14 @@
     <sheet name="004" sheetId="4" r:id="rId6"/>
     <sheet name="005" sheetId="8" r:id="rId7"/>
     <sheet name="006" sheetId="2" r:id="rId8"/>
+    <sheet name="007" sheetId="9" r:id="rId9"/>
+    <sheet name="008" sheetId="10" r:id="rId10"/>
+    <sheet name="009" sheetId="11" r:id="rId11"/>
+    <sheet name="010" sheetId="12" r:id="rId12"/>
+    <sheet name="011" sheetId="13" r:id="rId13"/>
+    <sheet name="012" sheetId="14" r:id="rId14"/>
+    <sheet name="013" sheetId="15" r:id="rId15"/>
+    <sheet name="014" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="42">
   <si>
     <t>Survey for Study</t>
   </si>
@@ -154,6 +162,21 @@
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>36-50</t>
+  </si>
+  <si>
+    <t>4 - Very rarely</t>
+  </si>
+  <si>
+    <t>Black or Black British – African</t>
+  </si>
+  <si>
+    <t>22-25</t>
+  </si>
+  <si>
+    <t>Asian or Asian British – Pakistani</t>
   </si>
 </sst>
 </file>
@@ -537,16 +560,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO15"/>
+  <dimension ref="A1:AO30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="62.5546875" style="12" customWidth="1"/>
-    <col min="2" max="8" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -574,14 +598,30 @@
       <c r="H1" s="8">
         <v>6</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="I1" s="8">
+        <v>7</v>
+      </c>
+      <c r="J1" s="8">
+        <v>8</v>
+      </c>
+      <c r="K1" s="8">
+        <v>9</v>
+      </c>
+      <c r="L1" s="8">
+        <v>10</v>
+      </c>
+      <c r="M1" s="8">
+        <v>11</v>
+      </c>
+      <c r="N1" s="8">
+        <v>12</v>
+      </c>
+      <c r="O1" s="8">
+        <v>13</v>
+      </c>
+      <c r="P1" s="8">
+        <v>14</v>
+      </c>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
@@ -640,6 +680,38 @@
         <f>IF(_xlfn.XLOOKUP($A2,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>Male</v>
       </c>
+      <c r="I2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>Female</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Male</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Male</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>Male</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Male</v>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Female</v>
+      </c>
+      <c r="O2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Female</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(_xlfn.XLOOKUP($A2,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A2,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Female</v>
+      </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -673,6 +745,38 @@
         <f>IF(_xlfn.XLOOKUP($A3,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>26-35</v>
       </c>
+      <c r="I3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>36-50</v>
+      </c>
+      <c r="J3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>36-50</v>
+      </c>
+      <c r="K3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>26-35</v>
+      </c>
+      <c r="L3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>36-50</v>
+      </c>
+      <c r="M3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>26-35</v>
+      </c>
+      <c r="N3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>36-50</v>
+      </c>
+      <c r="O3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>22-25</v>
+      </c>
+      <c r="P3" t="str">
+        <f>IF(_xlfn.XLOOKUP($A3,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A3,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>36-50</v>
+      </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -706,6 +810,38 @@
         <f>IF(_xlfn.XLOOKUP($A4,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>White – British</v>
       </c>
+      <c r="I4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>White – British</v>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>White – British</v>
+      </c>
+      <c r="K4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>White – British</v>
+      </c>
+      <c r="L4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>White – British</v>
+      </c>
+      <c r="M4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Black or Black British – African</v>
+      </c>
+      <c r="N4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>White – British</v>
+      </c>
+      <c r="O4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Asian or Asian British – Pakistani</v>
+      </c>
+      <c r="P4" t="str">
+        <f>IF(_xlfn.XLOOKUP($A4,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A4,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>White – British</v>
+      </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
@@ -739,6 +875,38 @@
         <f>IF(_xlfn.XLOOKUP($A5,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>Bachelor's degree with honours or equivalent</v>
       </c>
+      <c r="I5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>Bachelor's degree with honours or equivalent</v>
+      </c>
+      <c r="J5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Master's degree or equivalent</v>
+      </c>
+      <c r="K5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Bachelor's degree with honours or equivalent</v>
+      </c>
+      <c r="L5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>Bachelor's degree with honours or equivalent</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Master's degree or equivalent</v>
+      </c>
+      <c r="N5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Bachelor's degree with honours or equivalent</v>
+      </c>
+      <c r="O5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Bachelor's degree with honours or equivalent</v>
+      </c>
+      <c r="P5" t="str">
+        <f>IF(_xlfn.XLOOKUP($A5,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A5,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Master's degree or equivalent</v>
+      </c>
     </row>
     <row r="6" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
@@ -772,6 +940,38 @@
         <f>IF(_xlfn.XLOOKUP($A6,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v/>
       </c>
+      <c r="I6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="O6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <f>IF(_xlfn.XLOOKUP($A6,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A6,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -805,6 +1005,38 @@
         <f>IF(_xlfn.XLOOKUP($A7,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>Education</v>
       </c>
+      <c r="I7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="J7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="K7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="L7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="N7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="O7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
+      <c r="P7" t="str">
+        <f>IF(_xlfn.XLOOKUP($A7,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A7,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Information Technology (IT)</v>
+      </c>
     </row>
     <row r="8" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
@@ -838,6 +1070,38 @@
         <f>IF(_xlfn.XLOOKUP($A8,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v/>
       </c>
+      <c r="I8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <f>IF(_xlfn.XLOOKUP($A8,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A8,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
@@ -871,6 +1135,38 @@
         <f>IF(_xlfn.XLOOKUP($A9,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>No</v>
       </c>
+      <c r="I9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="J9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="K9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="L9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="M9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="N9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="O9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="P9" t="str">
+        <f>IF(_xlfn.XLOOKUP($A9,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A9,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
@@ -904,6 +1200,38 @@
         <f>IF(_xlfn.XLOOKUP($A10,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>No</v>
       </c>
+      <c r="I10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="J10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="K10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="L10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="M10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="N10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="O10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="P10" t="str">
+        <f>IF(_xlfn.XLOOKUP($A10,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A10,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -937,6 +1265,38 @@
         <f>IF(_xlfn.XLOOKUP($A11,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>5 - Never</v>
       </c>
+      <c r="I11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>5 - Never</v>
+      </c>
+      <c r="J11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>1 - Daily</v>
+      </c>
+      <c r="K11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>2 - Weekly</v>
+      </c>
+      <c r="L11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>5 - Never</v>
+      </c>
+      <c r="M11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>2 - Weekly</v>
+      </c>
+      <c r="N11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>4 - Very rarely</v>
+      </c>
+      <c r="O11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>5 - Never</v>
+      </c>
+      <c r="P11" t="str">
+        <f>IF(_xlfn.XLOOKUP($A11,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A11,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>1 - Daily</v>
+      </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
@@ -970,6 +1330,38 @@
         <f>IF(_xlfn.XLOOKUP($A12,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>Yes</v>
       </c>
+      <c r="I12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="J12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="K12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="L12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="M12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="N12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="O12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="P12" t="str">
+        <f>IF(_xlfn.XLOOKUP($A12,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A12,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
@@ -1003,6 +1395,38 @@
         <f>IF(_xlfn.XLOOKUP($A13,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>Yes</v>
       </c>
+      <c r="I13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="J13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="K13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="L13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>No</v>
+      </c>
+      <c r="M13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="N13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="O13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="P13" t="str">
+        <f>IF(_xlfn.XLOOKUP($A13,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A13,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
     </row>
     <row r="14" spans="1:41" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
@@ -1036,6 +1460,38 @@
         <f>IF(_xlfn.XLOOKUP($A14,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>1 - Daily</v>
       </c>
+      <c r="I14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>2 - Weekly</v>
+      </c>
+      <c r="J14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>1 - Daily</v>
+      </c>
+      <c r="K14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>2 - Weekly</v>
+      </c>
+      <c r="L14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>4 - Very rarely</v>
+      </c>
+      <c r="M14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>2 - Weekly</v>
+      </c>
+      <c r="N14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>1 - Daily</v>
+      </c>
+      <c r="O14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>3 - Monthly</v>
+      </c>
+      <c r="P14" t="str">
+        <f>IF(_xlfn.XLOOKUP($A14,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A14,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>1 - Daily</v>
+      </c>
     </row>
     <row r="15" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
@@ -1069,10 +1525,1305 @@
         <f>IF(_xlfn.XLOOKUP($A15,'006'!$B:$B,'006'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'006'!$B:$B,'006'!$C:$C,,0,1))</f>
         <v>Yes</v>
       </c>
+      <c r="I15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'007'!$B:$B,'007'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'007'!$B:$B,'007'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="J15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'008'!$B:$B,'008'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'008'!$B:$B,'008'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="K15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'009'!$B:$B,'009'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'009'!$B:$B,'009'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="L15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'010'!$B:$B,'010'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'010'!$B:$B,'010'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="M15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'011'!$B:$B,'011'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'011'!$B:$B,'011'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="N15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'012'!$B:$B,'012'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'012'!$B:$B,'012'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="O15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'013'!$B:$B,'013'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'013'!$B:$B,'013'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+      <c r="P15" t="str">
+        <f>IF(_xlfn.XLOOKUP($A15,'014'!$B:$B,'014'!$C:$C,,0,1)=0,"",_xlfn.XLOOKUP($A15,'014'!$B:$B,'014'!$C:$C,,0,1))</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+    </row>
+    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+    </row>
+    <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDB131-4B65-4720-990A-3A987A31EC6F}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CC61BA-C294-4BAC-8765-120DF329ED73}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6410A67-9EF2-4C9B-A396-78467ABEF985}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0754D71-3B55-41A2-A3E2-1AA721990C9F}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF122BE-C9F6-4CDF-AC1D-81BA66EDF3A0}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD698AE8-7C9A-4833-9C20-76F261E8F9E0}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BA0C1D-AF65-4295-812C-521B624D4100}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2307,4 +4058,181 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5611B4FC-B348-4AC1-A853-ADDC0EF215DA}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>